<commit_message>
Post DCT review with changes made to manuals and review version (before-acceptance) saved for all except CM since 'tracking' was not enabled. CM diff is a compare against 'indexed' version. Added DCT directory with filled in DCTs. Moved orginal DCTs to 'originals' directory. Next checkin will be clean up of review files to give a cleaner structure to the forms directories.
</commit_message>
<xml_diff>
--- a/FM/FM-Status.xlsx
+++ b/FM/FM-Status.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camroe/working/RepairServiceManual/FM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9373454C-0385-5742-B490-A050208CFA80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AE9FD26-9D2C-744F-B612-10F51F322640}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="460" windowWidth="27640" windowHeight="18540" xr2:uid="{6B23032B-54A6-D642-AD6D-9CF5C8532F8E}"/>
+    <workbookView xWindow="24260" yWindow="-18540" windowWidth="27640" windowHeight="18540" xr2:uid="{6B23032B-54A6-D642-AD6D-9CF5C8532F8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
   <si>
     <t>Form</t>
   </si>
@@ -158,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -166,17 +167,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
@@ -184,17 +201,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -242,16 +249,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -575,10 +572,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092F7872-07A1-3C42-8371-E23983A4A62B}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,367 +588,416 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="B22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="B24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="B25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" t="s">
-        <v>30</v>
-      </c>
+      <c r="B27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B27">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E27">
-    <cfRule type="containsBlanks" dxfId="5" priority="5">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C27">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Exists">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Exists">
       <formula>NOT(ISERROR(SEARCH("Exists",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D27">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E27">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -981,5 +1030,6 @@
     <hyperlink ref="A27" r:id="rId26" location="_Toc74055076" display="applewebdata://B361DA4F-9F99-447A-93F2-57541CDB7594/ - _Toc74055076" xr:uid="{EEEE85C3-FDD7-8C47-AEE1-8FD9419EEA3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="93" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>